<commit_message>
attempted more research; current thought for fifth table is a constellation table with cool facts
</commit_message>
<xml_diff>
--- a/Build a Celestial Bodies Database/Galaxies_db_info.xlsx
+++ b/Build a Celestial Bodies Database/Galaxies_db_info.xlsx
@@ -5,28 +5,29 @@
   <fileSharing readOnlyRecommended="0" userName="clkc6"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Galaxy" sheetId="1" r:id="rId4"/>
     <sheet name="Planet" sheetId="2" r:id="rId5"/>
     <sheet name="Star" sheetId="3" r:id="rId6"/>
     <sheet name="Moon" sheetId="4" r:id="rId7"/>
+    <sheet name="Constellation" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1719954588" val="1215" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1719954588" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1719954588"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1719954588"/>
+      <pm:revision xmlns:pm="smNativeData" day="1725394951" val="1215" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1725394951" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1725394951" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1725394951"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>galaxy_id</t>
   </si>
@@ -37,12 +38,12 @@
     <t>abbreviation</t>
   </si>
   <si>
+    <t>constellation</t>
+  </si>
+  <si>
     <t>distance_from_mw_in_kly</t>
   </si>
   <si>
-    <t>constellation</t>
-  </si>
-  <si>
     <t>size_in_ly</t>
   </si>
   <si>
@@ -52,18 +53,21 @@
     <t>shape</t>
   </si>
   <si>
+    <t>year_first_mentioned</t>
+  </si>
+  <si>
     <t>serial</t>
   </si>
   <si>
     <t>varchar(30)</t>
   </si>
   <si>
+    <t>varchar(60)/serial</t>
+  </si>
+  <si>
     <t>numeric(6,2)</t>
   </si>
   <si>
-    <t>varchar(60)</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -73,6 +77,9 @@
     <t>spiral, elliptical, irregular, lenticular(aka polar-ring)[, seyfert, quasars, blazars]</t>
   </si>
   <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>milky way</t>
   </si>
   <si>
@@ -205,19 +212,85 @@
     <t>exoplanet_classification</t>
   </si>
   <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
     <t>enum: DHJKLMNRTY</t>
   </si>
   <si>
+    <t>mercury</t>
+  </si>
+  <si>
+    <t>venus</t>
+  </si>
+  <si>
+    <t>earth</t>
+  </si>
+  <si>
+    <t>mars</t>
+  </si>
+  <si>
+    <t>jupiter</t>
+  </si>
+  <si>
+    <t>saturn</t>
+  </si>
+  <si>
+    <t>neptune</t>
+  </si>
+  <si>
+    <t>pluto</t>
+  </si>
+  <si>
+    <t>ceres</t>
+  </si>
+  <si>
+    <t>haumea</t>
+  </si>
+  <si>
+    <t>makemake</t>
+  </si>
+  <si>
+    <t>eris</t>
+  </si>
+  <si>
     <t>is_a_sun</t>
   </si>
   <si>
     <t>kind_of_star</t>
   </si>
   <si>
+    <t>size</t>
+  </si>
+  <si>
     <t>enum: GKM</t>
   </si>
   <si>
+    <t>numeric(4,2)</t>
+  </si>
+  <si>
     <t>moon_id</t>
+  </si>
+  <si>
+    <t>composition</t>
+  </si>
+  <si>
+    <t>varchar(16)</t>
+  </si>
+  <si>
+    <t>constellation_id</t>
+  </si>
+  <si>
+    <t>portrays</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>total_stars</t>
   </si>
 </sst>
 </file>
@@ -242,7 +315,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1719954588" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1725394951" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -257,7 +330,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1719954588" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1725394951" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -275,22 +348,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1719954588" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1719954588" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1725394951" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -301,7 +363,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1719954588" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1725394951" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -312,7 +374,18 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1719954588" type="1" fgLvl="50" fgClr="00FF00FF" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1725394951" type="1" fgLvl="50" fgClr="00FF00FF" bgLvl="50" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1725394951" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -334,7 +407,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1719954588"/>
+          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
         </ext>
       </extLst>
     </border>
@@ -353,7 +426,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1719954588"/>
+          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
         </ext>
       </extLst>
     </border>
@@ -372,7 +445,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1719954588"/>
+          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
         </ext>
       </extLst>
     </border>
@@ -391,7 +464,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1719954588"/>
+          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
         </ext>
       </extLst>
     </border>
@@ -410,7 +483,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1719954588"/>
+          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
         </ext>
       </extLst>
     </border>
@@ -418,12 +491,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -431,9 +508,13 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1719954588" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1725394951" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
+      <pm:colors xmlns:pm="smNativeData" id="1725394951" count="2">
+        <pm:color name="Color 24" rgb="A30000"/>
+        <pm:color name="Color 25" rgb="800180"/>
+      </pm:colors>
     </ext>
   </extLst>
 </styleSheet>
@@ -695,20 +776,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="2" max="2" width="20.945946" customWidth="1"/>
-    <col min="5" max="5" width="15.738739" customWidth="1"/>
+    <col min="4" max="4" width="15.738739" customWidth="1" style="6"/>
     <col min="7" max="7" width="10.000000" style="3"/>
+    <col min="8" max="8" width="33.936937" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -718,7 +800,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -733,234 +815,240 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
         <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="n">
         <v>2500</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>22000</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
+    </row>
+    <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:8">
       <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
       <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
+        <v>42</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
+        <v>43</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:8">
       <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="H16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
+        <v>46</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1719954588" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -969,16 +1057,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1719954588" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1719954588" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1719954588" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1719954588" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719954588" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -989,56 +1077,129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="3" max="3" width="10.000000" style="1"/>
+    <col min="5" max="5" width="19.801802" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1719954588" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1047,16 +1208,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1719954588" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1719954588" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1719954588" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1719954588" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719954588" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1067,20 +1228,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="3" max="3" width="10.000000" style="2"/>
+    <col min="5" max="5" width="10.621622" customWidth="1"/>
+    <col min="6" max="6" width="10.927928" customWidth="1"/>
+    <col min="7" max="7" width="10.810811" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1089,34 +1253,52 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1719954588" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1125,16 +1307,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1719954588" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1719954588" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1719954588" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1719954588" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719954588" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1145,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1156,33 +1338,48 @@
     <col min="3" max="3" width="10.000000" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1719954588" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1191,16 +1388,94 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1719954588" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1719954588" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1719954588" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1719954588" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1719954588" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
+  <cols>
+    <col min="1" max="1" width="13.207207" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
adding data points and expanding on table columns
</commit_message>
<xml_diff>
--- a/Build a Celestial Bodies Database/Galaxies_db_info.xlsx
+++ b/Build a Celestial Bodies Database/Galaxies_db_info.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="clkc6"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="3" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Galaxy" sheetId="1" r:id="rId4"/>
@@ -17,17 +17,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1725394951" val="1215" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1725394951" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1725394951" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1725394951"/>
+      <pm:revision xmlns:pm="smNativeData" day="1726260747" val="1215" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1726260747" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1726260747" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1726260747"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="130">
   <si>
     <t>galaxy_id</t>
   </si>
@@ -209,42 +209,81 @@
     <t>planet_type_by_composition</t>
   </si>
   <si>
+    <t>distance_from_star_in_U</t>
+  </si>
+  <si>
     <t>exoplanet_classification</t>
   </si>
   <si>
     <t>mass</t>
   </si>
   <si>
-    <t>radius</t>
+    <t>diameter_in_km</t>
+  </si>
+  <si>
+    <t>gravity</t>
+  </si>
+  <si>
+    <t>rings</t>
+  </si>
+  <si>
+    <t>total_moons</t>
   </si>
   <si>
     <t>enum: DHJKLMNRTY</t>
   </si>
   <si>
+    <t>numeric(9,0)</t>
+  </si>
+  <si>
     <t>mercury</t>
   </si>
   <si>
+    <t>terrestrial</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>venus</t>
   </si>
   <si>
     <t>earth</t>
   </si>
   <si>
+    <t>rock</t>
+  </si>
+  <si>
     <t>mars</t>
   </si>
   <si>
     <t>jupiter</t>
   </si>
   <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>giant</t>
+  </si>
+  <si>
     <t>saturn</t>
   </si>
   <si>
+    <t>uranus</t>
+  </si>
+  <si>
+    <t>ice</t>
+  </si>
+  <si>
     <t>neptune</t>
   </si>
   <si>
     <t>pluto</t>
   </si>
   <si>
+    <t>dwarf</t>
+  </si>
+  <si>
     <t>ceres</t>
   </si>
   <si>
@@ -275,10 +314,97 @@
     <t>moon_id</t>
   </si>
   <si>
+    <t>has_atmosphere</t>
+  </si>
+  <si>
+    <t>has_magnetic_field</t>
+  </si>
+  <si>
     <t>composition</t>
   </si>
   <si>
     <t>varchar(16)</t>
+  </si>
+  <si>
+    <t>https://science.nasa.gov/solar-system/moons/facts/</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Deimos</t>
+  </si>
+  <si>
+    <t>Phobos</t>
+  </si>
+  <si>
+    <t>Ganymede</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>Io</t>
+  </si>
+  <si>
+    <t>Dione</t>
+  </si>
+  <si>
+    <t>Saturn</t>
+  </si>
+  <si>
+    <t>Hyperion</t>
+  </si>
+  <si>
+    <t>Phoebe</t>
+  </si>
+  <si>
+    <t>Rhea</t>
+  </si>
+  <si>
+    <t>Titan</t>
+  </si>
+  <si>
+    <t>Ariel</t>
+  </si>
+  <si>
+    <t>Uranus</t>
+  </si>
+  <si>
+    <t>Oberon</t>
+  </si>
+  <si>
+    <t>Titania</t>
+  </si>
+  <si>
+    <t>Nereid</t>
+  </si>
+  <si>
+    <t>Neptune</t>
+  </si>
+  <si>
+    <t>Triton</t>
+  </si>
+  <si>
+    <t>Charon</t>
+  </si>
+  <si>
+    <t>Pluto</t>
+  </si>
+  <si>
+    <t>Dysnomia</t>
+  </si>
+  <si>
+    <t>Eris</t>
+  </si>
+  <si>
+    <t>Namaka</t>
+  </si>
+  <si>
+    <t>Haumea</t>
+  </si>
+  <si>
+    <t>Hi'iaka</t>
   </si>
   <si>
     <t>constellation_id</t>
@@ -315,7 +441,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1725394951" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1726260747" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -330,7 +456,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1725394951" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1726260747" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -352,7 +478,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1725394951" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1726260747" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -363,7 +489,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1725394951" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1726260747" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -374,7 +500,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1725394951" type="1" fgLvl="50" fgClr="00FF00FF" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1726260747" type="1" fgLvl="50" fgClr="00FF00FF" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -385,7 +511,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1725394951" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1726260747" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -407,7 +533,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
+          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
         </ext>
       </extLst>
     </border>
@@ -426,7 +552,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
+          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
         </ext>
       </extLst>
     </border>
@@ -445,7 +571,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
+          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
         </ext>
       </extLst>
     </border>
@@ -464,7 +590,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
+          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
         </ext>
       </extLst>
     </border>
@@ -483,7 +609,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1725394951"/>
+          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
         </ext>
       </extLst>
     </border>
@@ -491,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
@@ -500,7 +626,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -508,10 +633,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1725394951" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1726260747" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1725394951" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1726260747" count="2">
         <pm:color name="Color 24" rgb="A30000"/>
         <pm:color name="Color 25" rgb="800180"/>
       </pm:colors>
@@ -785,7 +910,7 @@
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="2" max="2" width="20.945946" customWidth="1"/>
-    <col min="4" max="4" width="15.738739" customWidth="1" style="6"/>
+    <col min="4" max="4" width="15.738739" customWidth="1" style="1"/>
     <col min="7" max="7" width="10.000000" style="3"/>
     <col min="8" max="8" width="33.936937" customWidth="1"/>
   </cols>
@@ -800,7 +925,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -829,7 +954,7 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
@@ -852,7 +977,7 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H3" t="s">
@@ -863,7 +988,7 @@
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="n">
@@ -883,7 +1008,7 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -891,7 +1016,7 @@
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -899,7 +1024,7 @@
       <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H7" t="s">
@@ -910,7 +1035,7 @@
       <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -918,7 +1043,7 @@
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -926,7 +1051,7 @@
       <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -934,7 +1059,7 @@
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="H11" t="s">
@@ -948,7 +1073,7 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -962,7 +1087,7 @@
       <c r="C13" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -973,7 +1098,7 @@
       <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -981,7 +1106,7 @@
       <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -989,7 +1114,7 @@
       <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H16" t="s">
@@ -1000,7 +1125,7 @@
       <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1008,7 +1133,7 @@
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1016,7 +1141,7 @@
       <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1048,7 +1173,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1057,16 +1182,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1077,19 +1202,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="3" max="3" width="10.000000" style="1"/>
-    <col min="5" max="5" width="19.801802" customWidth="1"/>
+    <col min="4" max="4" width="23.621622" customWidth="1"/>
+    <col min="5" max="5" width="21.936937" customWidth="1"/>
+    <col min="6" max="6" width="19.801802" customWidth="1"/>
+    <col min="8" max="8" width="13.621622" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1112,10 +1240,22 @@
         <v>62</v>
       </c>
       <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1129,77 +1269,238 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
       </c>
       <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" t="n">
+        <v>139822</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" t="n">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1740</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2003</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="n">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>75</v>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2400</v>
+      </c>
+      <c r="K15" t="s">
+        <v>71</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1208,16 +1509,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1231,7 +1532,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1253,13 +1554,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="F1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1282,10 +1583,10 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -1298,7 +1599,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1307,16 +1608,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1327,20 +1628,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="3" max="3" width="10.000000" style="2"/>
+    <col min="4" max="5" width="13.621622" customWidth="1"/>
+    <col min="6" max="6" width="16.315315" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1349,16 +1652,22 @@
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1368,18 +1677,308 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" t="s">
         <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3471</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="n">
+        <v>17.3999999999999986</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <f>2631*2</f>
+        <v>5262</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1388,16 +1987,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1421,19 +2020,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
@@ -1457,7 +2056,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1725394951" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1466,16 +2065,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1725394951" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1725394951" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1725394951" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Adding more values and details to Constellation, updating Umlet to include new table Constellation
</commit_message>
<xml_diff>
--- a/Build a Celestial Bodies Database/Galaxies_db_info.xlsx
+++ b/Build a Celestial Bodies Database/Galaxies_db_info.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="clkc6"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="4" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Galaxy" sheetId="1" r:id="rId4"/>
@@ -17,17 +17,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1726260747" val="1215" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1726260747" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1726260747" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1726260747"/>
+      <pm:revision xmlns:pm="smNativeData" day="1729191607" val="1215" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1729191607" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1729191607" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1729191607"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="189">
   <si>
     <t>galaxy_id</t>
   </si>
@@ -182,6 +182,12 @@
     <t>whirlpool galaxy</t>
   </si>
   <si>
+    <t>gliese 667</t>
+  </si>
+  <si>
+    <t>scorpio</t>
+  </si>
+  <si>
     <t>listing names &amp; constellations</t>
   </si>
   <si>
@@ -224,6 +230,9 @@
     <t>gravity</t>
   </si>
   <si>
+    <t>habitable</t>
+  </si>
+  <si>
     <t>rings</t>
   </si>
   <si>
@@ -236,9 +245,15 @@
     <t>numeric(9,0)</t>
   </si>
   <si>
+    <t>YMN</t>
+  </si>
+  <si>
     <t>mercury</t>
   </si>
   <si>
+    <t>Sol</t>
+  </si>
+  <si>
     <t>terrestrial</t>
   </si>
   <si>
@@ -254,9 +269,15 @@
     <t>rock</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>mars</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>jupiter</t>
   </si>
   <si>
@@ -296,6 +317,33 @@
     <t>eris</t>
   </si>
   <si>
+    <t>gliese 667 cb</t>
+  </si>
+  <si>
+    <t>gj 667c</t>
+  </si>
+  <si>
+    <t>gliese 667 cc</t>
+  </si>
+  <si>
+    <t>gliese 667 ce</t>
+  </si>
+  <si>
+    <t>gliese 667 cf</t>
+  </si>
+  <si>
+    <t>kepler 452b</t>
+  </si>
+  <si>
+    <t>TOI-715 b</t>
+  </si>
+  <si>
+    <t>TOI-715</t>
+  </si>
+  <si>
+    <t>GJ 9827d</t>
+  </si>
+  <si>
     <t>is_a_sun</t>
   </si>
   <si>
@@ -311,6 +359,21 @@
     <t>numeric(4,2)</t>
   </si>
   <si>
+    <t>GJ 667 A</t>
+  </si>
+  <si>
+    <t>K-type</t>
+  </si>
+  <si>
+    <t>GJ 667 B</t>
+  </si>
+  <si>
+    <t>GJ 667 C</t>
+  </si>
+  <si>
+    <t>sol</t>
+  </si>
+  <si>
     <t>moon_id</t>
   </si>
   <si>
@@ -410,13 +473,127 @@
     <t>constellation_id</t>
   </si>
   <si>
-    <t>portrays</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
     <t>total_stars</t>
+  </si>
+  <si>
+    <t>https://starchild.gsfc.nasa.gov/docs/StarChild/questions/88constellations.html</t>
+  </si>
+  <si>
+    <t>sagittarius</t>
+  </si>
+  <si>
+    <t>Archer</t>
+  </si>
+  <si>
+    <t>Princess of Ethiopia</t>
+  </si>
+  <si>
+    <t>Berenice's hair</t>
+  </si>
+  <si>
+    <t>Big bear</t>
+  </si>
+  <si>
+    <t>Sculptor's tools</t>
+  </si>
+  <si>
+    <t>Sextant</t>
+  </si>
+  <si>
+    <t>serpens</t>
+  </si>
+  <si>
+    <t>Serpent</t>
+  </si>
+  <si>
+    <t>Swordfish</t>
+  </si>
+  <si>
+    <t>Toucan</t>
+  </si>
+  <si>
+    <t>Virgin</t>
+  </si>
+  <si>
+    <t>Hunting dogs</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>scorpius</t>
+  </si>
+  <si>
+    <t>Scorpion</t>
+  </si>
+  <si>
+    <t>Cassiopeia</t>
+  </si>
+  <si>
+    <t>Queen of Ethiopia</t>
+  </si>
+  <si>
+    <t>ursa minor</t>
+  </si>
+  <si>
+    <t>Little bear</t>
+  </si>
+  <si>
+    <t>Aquarius</t>
+  </si>
+  <si>
+    <t>Water bearer</t>
+  </si>
+  <si>
+    <t>aries</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>taurus</t>
+  </si>
+  <si>
+    <t>Bull</t>
+  </si>
+  <si>
+    <t>gemini</t>
+  </si>
+  <si>
+    <t>Twins</t>
+  </si>
+  <si>
+    <t>cancer</t>
+  </si>
+  <si>
+    <t>Crab</t>
+  </si>
+  <si>
+    <t>leo</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>libra</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>capricorn</t>
+  </si>
+  <si>
+    <t>Sea Goat</t>
+  </si>
+  <si>
+    <t>pisces</t>
+  </si>
+  <si>
+    <t>Fishes</t>
   </si>
 </sst>
 </file>
@@ -441,7 +618,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1726260747" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1729191607" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -456,7 +633,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1726260747" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1729191607" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -478,7 +655,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1726260747" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1729191607" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -489,7 +666,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1726260747" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1729191607" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -500,7 +677,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1726260747" type="1" fgLvl="50" fgClr="00FF00FF" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1729191607" type="1" fgLvl="50" fgClr="00FF00FF" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -511,7 +688,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1726260747" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1729191607" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -533,7 +710,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
+          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
         </ext>
       </extLst>
     </border>
@@ -552,7 +729,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
+          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
         </ext>
       </extLst>
     </border>
@@ -571,7 +748,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
+          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
         </ext>
       </extLst>
     </border>
@@ -590,7 +767,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
+          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
         </ext>
       </extLst>
     </border>
@@ -609,7 +786,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1726260747"/>
+          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
         </ext>
       </extLst>
     </border>
@@ -617,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
@@ -626,6 +803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -633,10 +811,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1726260747" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1729191607" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1726260747" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1729191607" count="2">
         <pm:color name="Color 24" rgb="A30000"/>
         <pm:color name="Color 25" rgb="800180"/>
       </pm:colors>
@@ -904,7 +1082,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D2" sqref="D2:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1145,35 +1323,43 @@
         <v>47</v>
       </c>
     </row>
+    <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1182,16 +1368,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1202,14 +1388,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
+    <col min="2" max="2" width="11.414414" customWidth="1"/>
     <col min="3" max="3" width="10.000000" style="1"/>
     <col min="4" max="4" width="23.621622" customWidth="1"/>
     <col min="5" max="5" width="21.936937" customWidth="1"/>
@@ -1217,45 +1404,48 @@
     <col min="8" max="8" width="13.621622" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>65</v>
-      </c>
       <c r="L1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>68</v>
+      </c>
+      <c r="M1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1272,235 +1462,336 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:13">
       <c r="B3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K3" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" t="n">
+        <v>75</v>
+      </c>
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:13">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" t="n">
+        <v>75</v>
+      </c>
+      <c r="L4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:13">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>78</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
-      <c r="K5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12">
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" t="s">
         <v>75</v>
       </c>
-      <c r="D6" t="s">
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="H7" t="n">
         <v>139822</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>21</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:13">
       <c r="B8" t="s">
-        <v>79</v>
+        <v>86</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" t="s">
         <v>21</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:13">
       <c r="B9" t="s">
-        <v>80</v>
+        <v>87</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" t="s">
         <v>21</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:13">
       <c r="B10" t="s">
-        <v>82</v>
+        <v>89</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
-      </c>
-      <c r="K10" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" t="s">
         <v>21</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:13">
       <c r="B11" t="s">
-        <v>83</v>
+        <v>90</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" t="s">
-        <v>71</v>
-      </c>
-      <c r="L11" t="n">
+        <v>91</v>
+      </c>
+      <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>85</v>
+        <v>92</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E13" t="n">
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H13" t="n">
         <v>1740</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>2003</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>21</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:13">
       <c r="B14" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
-      </c>
-      <c r="L14" t="n">
+        <v>91</v>
+      </c>
+      <c r="M14" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:13">
       <c r="B15" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E15" t="n">
         <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H15" t="n">
         <v>2400</v>
       </c>
-      <c r="K15" t="s">
-        <v>71</v>
-      </c>
-      <c r="L15" t="n">
+      <c r="L15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" t="s">
+        <v>100</v>
+      </c>
+      <c r="J19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+      <c r="K22" t="n">
+        <v>2017</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1509,16 +1800,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1529,10 +1820,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1545,7 +1836,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1554,13 +1845,13 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="F1" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1583,23 +1874,81 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1608,16 +1957,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1630,7 +1979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -1643,25 +1992,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="G1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1687,41 +2036,41 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D3" t="n">
         <v>3471</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D4" t="n">
-        <v>17.3999999999999986</v>
+        <v>17.399999999999995</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H4" t="n">
         <v>1877</v>
@@ -1729,13 +2078,13 @@
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H5" t="n">
         <v>1877</v>
@@ -1743,10 +2092,10 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D6">
         <f>2631*2</f>
@@ -1761,13 +2110,13 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
         <v>76</v>
-      </c>
-      <c r="F7" t="s">
-        <v>71</v>
       </c>
       <c r="H7" t="n">
         <v>1610</v>
@@ -1775,13 +2124,13 @@
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
         <v>76</v>
-      </c>
-      <c r="F8" t="s">
-        <v>71</v>
       </c>
       <c r="H8" t="n">
         <v>1610</v>
@@ -1789,13 +2138,13 @@
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H9" t="n">
         <v>1684</v>
@@ -1803,13 +2152,13 @@
     </row>
     <row r="10" spans="2:8">
       <c r="B10" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H10" t="n">
         <v>1848</v>
@@ -1817,13 +2166,13 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H11" t="n">
         <v>1898</v>
@@ -1831,13 +2180,13 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H12" t="n">
         <v>1672</v>
@@ -1845,13 +2194,13 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H13" t="n">
         <v>1655</v>
@@ -1859,13 +2208,13 @@
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H14" t="n">
         <v>1851</v>
@@ -1873,13 +2222,13 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H15" t="n">
         <v>1787</v>
@@ -1887,13 +2236,13 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="F16" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H16" t="n">
         <v>1787</v>
@@ -1901,13 +2250,13 @@
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H17" t="n">
         <v>1949</v>
@@ -1915,13 +2264,13 @@
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H18" t="n">
         <v>1846</v>
@@ -1929,13 +2278,13 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H19" t="n">
         <v>1978</v>
@@ -1943,42 +2292,42 @@
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="F22" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1987,16 +2336,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2007,56 +2356,261 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="13.207207" customWidth="1"/>
+    <col min="1" max="1" width="13.558559" customWidth="1"/>
+    <col min="2" max="2" width="14.828829" customWidth="1"/>
+    <col min="3" max="3" width="16.720721" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
         <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1726260747" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2065,16 +2619,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1726260747" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1726260747" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1726260747" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Update checklist of requirements; add details to excel doc & organize columns for final db columns
</commit_message>
<xml_diff>
--- a/Build a Celestial Bodies Database/Galaxies_db_info.xlsx
+++ b/Build a Celestial Bodies Database/Galaxies_db_info.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="clkc6"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Galaxy" sheetId="1" r:id="rId4"/>
@@ -17,17 +17,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1729191607" val="1215" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1729191607" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1729191607" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1729191607"/>
+      <pm:revision xmlns:pm="smNativeData" day="1733801907" val="1215" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1733801907" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1733801907" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1733801907"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="192">
   <si>
     <t>galaxy_id</t>
   </si>
@@ -59,6 +59,9 @@
     <t>serial</t>
   </si>
   <si>
+    <t>varchar(30) unique</t>
+  </si>
+  <si>
     <t>varchar(30)</t>
   </si>
   <si>
@@ -215,6 +218,15 @@
     <t>planet_type_by_composition</t>
   </si>
   <si>
+    <t>rings</t>
+  </si>
+  <si>
+    <t>total_moons</t>
+  </si>
+  <si>
+    <t>habitable</t>
+  </si>
+  <si>
     <t>distance_from_star_in_U</t>
   </si>
   <si>
@@ -230,13 +242,7 @@
     <t>gravity</t>
   </si>
   <si>
-    <t>habitable</t>
-  </si>
-  <si>
-    <t>rings</t>
-  </si>
-  <si>
-    <t>total_moons</t>
+    <t>YMN</t>
   </si>
   <si>
     <t>enum: DHJKLMNRTY</t>
@@ -245,21 +251,18 @@
     <t>numeric(9,0)</t>
   </si>
   <si>
-    <t>YMN</t>
-  </si>
-  <si>
     <t>mercury</t>
   </si>
   <si>
     <t>Sol</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
     <t>terrestrial</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>venus</t>
   </si>
   <si>
@@ -476,7 +479,10 @@
     <t>description</t>
   </si>
   <si>
-    <t>total_stars</t>
+    <t>main_stars</t>
+  </si>
+  <si>
+    <t>part_of_zodiac</t>
   </si>
   <si>
     <t>https://starchild.gsfc.nasa.gov/docs/StarChild/questions/88constellations.html</t>
@@ -485,7 +491,7 @@
     <t>sagittarius</t>
   </si>
   <si>
-    <t>Archer</t>
+    <t>Centaur / Archer</t>
   </si>
   <si>
     <t>Princess of Ethiopia</t>
@@ -581,7 +587,7 @@
     <t>libra</t>
   </si>
   <si>
-    <t>Balance</t>
+    <t>Scales / Balance</t>
   </si>
   <si>
     <t>capricorn</t>
@@ -593,7 +599,10 @@
     <t>pisces</t>
   </si>
   <si>
-    <t>Fishes</t>
+    <t>Two Fishes</t>
+  </si>
+  <si>
+    <t>https://www.universeguide.com/blogarticle/list-of-constellations-ordered-by-main-star-count-smallest-to-largest</t>
   </si>
 </sst>
 </file>
@@ -618,7 +627,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1729191607" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1733801907" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -633,7 +642,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1729191607" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1733801907" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -642,7 +651,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -655,7 +664,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1729191607" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1733801907" type="1" fgLvl="100" fgClr="00FF0000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -666,7 +675,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1729191607" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1733801907" type="1" fgLvl="64" fgClr="00FF0000" bgLvl="36" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -677,7 +686,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1729191607" type="1" fgLvl="50" fgClr="00FF00FF" bgLvl="50" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1733801907" type="1" fgLvl="50" fgClr="00FF00FF" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -688,13 +697,24 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1729191607" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1733801907" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800101"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1733801907" type="1" fgLvl="50" fgClr="00FF0000" bgLvl="50" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -710,7 +730,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
+          <pm:border xmlns:pm="smNativeData" id="1733801907"/>
         </ext>
       </extLst>
     </border>
@@ -729,7 +749,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
+          <pm:border xmlns:pm="smNativeData" id="1733801907"/>
         </ext>
       </extLst>
     </border>
@@ -748,7 +768,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
+          <pm:border xmlns:pm="smNativeData" id="1733801907"/>
         </ext>
       </extLst>
     </border>
@@ -767,7 +787,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
+          <pm:border xmlns:pm="smNativeData" id="1733801907"/>
         </ext>
       </extLst>
     </border>
@@ -786,7 +806,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1729191607"/>
+          <pm:border xmlns:pm="smNativeData" id="1733801907"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1733801907"/>
         </ext>
       </extLst>
     </border>
@@ -803,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -811,10 +850,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1729191607" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1733801907" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1729191607" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1733801907" count="2">
         <pm:color name="Color 24" rgb="A30000"/>
         <pm:color name="Color 25" rgb="800180"/>
       </pm:colors>
@@ -1082,7 +1121,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D20"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1130,44 +1169,44 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" t="n">
         <v>2500</v>
@@ -1176,190 +1215,190 @@
         <v>22000</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:8">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:8">
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1733801907" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1368,16 +1407,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1733801907" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1388,402 +1427,403 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="2" max="2" width="11.414414" customWidth="1"/>
-    <col min="3" max="3" width="10.000000" style="1"/>
+    <col min="3" max="3" width="10.000000" style="2"/>
     <col min="4" max="4" width="23.621622" customWidth="1"/>
-    <col min="5" max="5" width="21.936937" customWidth="1"/>
-    <col min="6" max="6" width="19.801802" customWidth="1"/>
-    <col min="8" max="8" width="13.621622" customWidth="1"/>
+    <col min="6" max="6" width="10.621622" customWidth="1"/>
+    <col min="8" max="8" width="21.936937" customWidth="1"/>
+    <col min="9" max="9" width="19.801802" customWidth="1"/>
+    <col min="11" max="11" width="13.621622" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
+      <c r="C1" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
         <v>72</v>
       </c>
       <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="n">
+        <v>95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" t="n">
+        <v>139822</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="n">
+        <v>146</v>
+      </c>
+      <c r="I8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="n">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="n">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13">
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="I10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L3" t="s">
+      <c r="E11" t="s">
         <v>76</v>
       </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13">
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F11" t="n">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L4" t="s">
+      <c r="I12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" t="n">
+        <v>43</v>
+      </c>
+      <c r="I13" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1740</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
         <v>76</v>
       </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13">
-      <c r="B5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" t="s">
-        <v>80</v>
-      </c>
-      <c r="L5" t="s">
-        <v>76</v>
-      </c>
-      <c r="M5" t="n">
+      <c r="F15" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:13">
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" t="s">
-        <v>76</v>
-      </c>
-      <c r="M6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13">
-      <c r="B7" t="s">
+      <c r="H15" t="n">
+        <v>68</v>
+      </c>
+      <c r="I15" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" t="n">
-        <v>139822</v>
-      </c>
-      <c r="L7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13">
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" t="s">
-        <v>85</v>
-      </c>
-      <c r="L8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" t="n">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13">
-      <c r="B9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" t="s">
-        <v>85</v>
-      </c>
-      <c r="L9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13">
-      <c r="B10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" t="s">
-        <v>85</v>
-      </c>
-      <c r="L10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13">
-      <c r="B11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" t="s">
-        <v>91</v>
-      </c>
-      <c r="L11" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13">
-      <c r="B13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" t="n">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1740</v>
-      </c>
-      <c r="K13" t="n">
-        <v>2003</v>
-      </c>
-      <c r="L13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13">
-      <c r="B14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" t="s">
-        <v>91</v>
-      </c>
-      <c r="M14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13">
-      <c r="B15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" t="n">
-        <v>68</v>
-      </c>
-      <c r="F15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" t="n">
-        <v>2400</v>
-      </c>
-      <c r="L15" t="s">
-        <v>76</v>
-      </c>
-      <c r="M15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10">
+    </row>
+    <row r="17" spans="2:7">
       <c r="B17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
       <c r="B18" t="s">
-        <v>99</v>
-      </c>
-      <c r="J18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
+        <v>100</v>
+      </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
       <c r="B19" t="s">
-        <v>100</v>
-      </c>
-      <c r="J19" t="s">
-        <v>82</v>
+        <v>101</v>
+      </c>
+      <c r="G19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
       <c r="B21" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="C21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="B22" t="s">
-        <v>104</v>
-      </c>
-      <c r="K22" t="n">
+        <v>105</v>
+      </c>
+      <c r="N22" t="n">
         <v>2017</v>
       </c>
     </row>
@@ -1791,7 +1831,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1733801907" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1800,16 +1840,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1733801907" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1823,20 +1863,21 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
+    <col min="2" max="2" width="15.927928" customWidth="1"/>
     <col min="3" max="3" width="10.000000" style="2"/>
     <col min="5" max="5" width="10.621622" customWidth="1"/>
     <col min="6" max="6" width="10.927928" customWidth="1"/>
-    <col min="7" max="7" width="10.810811" customWidth="1"/>
+    <col min="7" max="7" width="10.810811" customWidth="1" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1845,15 +1886,15 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
@@ -1871,84 +1912,84 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
         <v>112</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1733801907" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1957,16 +1998,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1733801907" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1980,11 +2021,12 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
+    <col min="2" max="2" width="15.927928" customWidth="1"/>
     <col min="3" max="3" width="10.000000" style="2"/>
     <col min="4" max="5" width="13.621622" customWidth="1"/>
     <col min="6" max="6" width="16.315315" customWidth="1"/>
@@ -1992,25 +2034,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -2027,30 +2069,30 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D3" t="n">
         <v>3471</v>
@@ -2061,10 +2103,10 @@
     </row>
     <row r="4" spans="2:8">
       <c r="B4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D4" t="n">
         <v>17.399999999999995</v>
@@ -2078,10 +2120,10 @@
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
         <v>76</v>
@@ -2092,17 +2134,17 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D6">
         <f>2631*2</f>
         <v>5262</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" t="n">
         <v>1610</v>
@@ -2110,10 +2152,10 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
         <v>76</v>
@@ -2124,10 +2166,10 @@
     </row>
     <row r="8" spans="2:8">
       <c r="B8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
         <v>76</v>
@@ -2138,10 +2180,10 @@
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F9" t="s">
         <v>76</v>
@@ -2152,10 +2194,10 @@
     </row>
     <row r="10" spans="2:8">
       <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="F10" t="s">
         <v>76</v>
@@ -2166,10 +2208,10 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F11" t="s">
         <v>76</v>
@@ -2180,10 +2222,10 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F12" t="s">
         <v>76</v>
@@ -2194,10 +2236,10 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F13" t="s">
         <v>76</v>
@@ -2208,10 +2250,10 @@
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F14" t="s">
         <v>76</v>
@@ -2222,10 +2264,10 @@
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="F15" t="s">
         <v>76</v>
@@ -2236,10 +2278,10 @@
     </row>
     <row r="16" spans="2:8">
       <c r="B16" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F16" t="s">
         <v>76</v>
@@ -2250,10 +2292,10 @@
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F17" t="s">
         <v>76</v>
@@ -2264,10 +2306,10 @@
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="F18" t="s">
         <v>76</v>
@@ -2278,10 +2320,10 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F19" t="s">
         <v>76</v>
@@ -2292,10 +2334,10 @@
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F20" t="s">
         <v>76</v>
@@ -2303,10 +2345,10 @@
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F21" t="s">
         <v>76</v>
@@ -2314,10 +2356,10 @@
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="F22" t="s">
         <v>76</v>
@@ -2327,7 +2369,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1733801907" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2336,16 +2378,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1733801907" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2356,34 +2398,37 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="1" max="1" width="13.558559" customWidth="1"/>
-    <col min="2" max="2" width="14.828829" customWidth="1"/>
+    <col min="2" max="2" width="15.927928" customWidth="1"/>
     <col min="3" max="3" width="16.720721" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2394,223 +2439,330 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:2">
-      <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="6" t="s">
-        <v>151</v>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
+        <v>153</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>154</v>
+      </c>
+      <c r="D4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="6" t="s">
-        <v>20</v>
+      <c r="B5" t="s">
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D5" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="6" t="s">
-        <v>23</v>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>156</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>157</v>
+      </c>
+      <c r="D7" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>158</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
+        <v>160</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="6" t="s">
-        <v>38</v>
+        <v>161</v>
+      </c>
+      <c r="D10" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" t="s">
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>162</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="6" t="s">
-        <v>45</v>
+        <v>163</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="6" t="s">
-        <v>47</v>
+        <v>164</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>165</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="D15" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" t="s">
+        <v>167</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>168</v>
+      </c>
+      <c r="D16" t="n">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D17" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
+        <v>172</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
+        <v>174</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
+        <v>176</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
+        <v>178</v>
+      </c>
+      <c r="D21" t="n">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
+        <v>180</v>
+      </c>
+      <c r="D22" t="n">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
       <c r="B23" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C23" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
+        <v>182</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
       <c r="B24" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C24" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
+        <v>184</v>
+      </c>
+      <c r="D24" t="n">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
       <c r="B25" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
+        <v>186</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
       <c r="B26" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
+        <v>188</v>
+      </c>
+      <c r="D26" t="n">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
       <c r="B27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C27" t="s">
-        <v>188</v>
+        <v>190</v>
+      </c>
+      <c r="D27" t="n">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1729191607" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1733801907" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2619,16 +2771,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1729191607" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1729191607" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1733801907" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1733801907" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1729191607" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1733801907" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>